<commit_message>
Updated Daily Activity Tracker for Today
</commit_message>
<xml_diff>
--- a/Daily Activity Tracker/Daily_Activity_Tracker_August.xlsx
+++ b/Daily Activity Tracker/Daily_Activity_Tracker_August.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chandrakanb\chandrakanb\Daily Activity Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B8B508-D3C5-4E66-AD72-827025F75C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2193122A-FA47-4AF4-9563-67D54B543B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day_month" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t xml:space="preserve">Sr.No. </t>
   </si>
@@ -110,13 +110,16 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Calibration</t>
-  </si>
-  <si>
-    <t>New TS Creation</t>
-  </si>
-  <si>
-    <t>A14 Fixation</t>
+    <t>Calibration on Bench 09.</t>
+  </si>
+  <si>
+    <t>Overnight Execution Fixation for Bench 09</t>
+  </si>
+  <si>
+    <t>New Test Script Developmenton Bench 09</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
   </si>
 </sst>
 </file>
@@ -322,70 +325,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -898,13 +838,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>SEARCH("In-Progress", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>SEARCH("Incomplete", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>SEARCH("Completed", D1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1076,26 +1016,15 @@
       <c r="D12" s="13"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1 D12:D1048576">
-    <cfRule type="expression" dxfId="17" priority="7">
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>SEARCH("In-Progress", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="8">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>SEARCH("Incomplete", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>SEARCH("Completed", D1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D11">
-    <cfRule type="expression" dxfId="14" priority="1">
-      <formula>SEARCH("In-Progress", D2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
-      <formula>SEARCH("Incomplete", D2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
-      <formula>SEARCH("Completed", D2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1107,7 +1036,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D12"/>
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1286,37 +1215,15 @@
       <c r="D13" s="13"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1 D14:D1048576">
-    <cfRule type="expression" dxfId="11" priority="7">
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>SEARCH("In-Progress", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>SEARCH("Incomplete", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>SEARCH("Completed", D1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>SEARCH("In-Progress", D13)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>SEARCH("Incomplete", D13)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>SEARCH("Completed", D13)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D12">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>SEARCH("In-Progress", D2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>SEARCH("Incomplete", D2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>SEARCH("Completed", D2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1325,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F135802-11A8-408F-949F-A2C0D125685D}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1357,43 +1264,61 @@
         <f t="shared" ref="A2:A11" si="0">ROW() - ROW($A$1)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
     </row>
@@ -1429,7 +1354,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
@@ -1438,7 +1365,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
     </row>
@@ -1452,21 +1381,6 @@
         <v>0</v>
       </c>
       <c r="D12" s="13"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>

<commit_message>
modified:   Daily Activity Tracker/Daily_Activity_Tracker_August.xlsx
</commit_message>
<xml_diff>
--- a/Daily Activity Tracker/Daily_Activity_Tracker_August.xlsx
+++ b/Daily Activity Tracker/Daily_Activity_Tracker_August.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chandrakanb\chandrakanb\Daily Activity Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2193122A-FA47-4AF4-9563-67D54B543B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757C8288-A19E-4EA3-82C8-41022E0F6E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day_month" sheetId="1" r:id="rId1"/>
     <sheet name="1st_August" sheetId="2" r:id="rId2"/>
     <sheet name="2nd_August" sheetId="3" r:id="rId3"/>
-    <sheet name="5th_August" sheetId="5" r:id="rId4"/>
+    <sheet name="5th_August" sheetId="4" r:id="rId4"/>
+    <sheet name="6th_August" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,35 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BA31306B-EA19-4EFA-B736-A30B21B9E199}</author>
+    <author>tc={22B59C60-CA0F-476C-B8F5-61A5244C0E0A}</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{BA31306B-EA19-4EFA-B736-A30B21B9E199}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Mute State Validation Issue Resolved with the help of Sahil on Bench 09, and the Appium issue resolved on Bench 06.</t>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{22B59C60-CA0F-476C-B8F5-61A5244C0E0A}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
   <si>
     <t xml:space="preserve">Sr.No. </t>
   </si>
@@ -47,12 +75,18 @@
     <t>Time Taken</t>
   </si>
   <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
     <t>Fixed the Mute State Validation Issue on the Bench 09.</t>
   </si>
   <si>
+    <t>Completed</t>
+  </si>
+  <si>
     <t>Added Auto Flashing TYAW Pack to OBU_A14_Repo.</t>
   </si>
   <si>
@@ -104,22 +138,34 @@
     <t>Performed sanity of the Bench 09.</t>
   </si>
   <si>
-    <t xml:space="preserve">Status </t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>Calibration on Bench 09.</t>
   </si>
   <si>
     <t>Overnight Execution Fixation for Bench 09</t>
   </si>
   <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
     <t>New Test Script Developmenton Bench 09</t>
   </si>
   <si>
-    <t>In-Progress</t>
+    <t>Overnight execution analysis of Bench 06.</t>
+  </si>
+  <si>
+    <t>Published the overnight execution reports of Bench 09.</t>
+  </si>
+  <si>
+    <t>Published the overnight execution reports of Bench 06.</t>
+  </si>
+  <si>
+    <t>Overnight Execution Fixation for Bench 09 and Bench 06.</t>
+  </si>
+  <si>
+    <t>Performed GIT Pull on Bench 06.</t>
+  </si>
+  <si>
+    <t>Performed sanity of the Bench 06.</t>
   </si>
 </sst>
 </file>
@@ -325,7 +371,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -421,6 +488,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Chandrakant Bhalekar" id="{124407F7-A124-478C-91FF-291E9D96DE6A}" userId="S::chandrakanb@kpit.com::fbaa0227-8d16-4af9-aaf0-17c8889162fe" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -706,12 +779,24 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B6" dT="2024-08-06T14:42:00.41" personId="{124407F7-A124-478C-91FF-291E9D96DE6A}" id="{BA31306B-EA19-4EFA-B736-A30B21B9E199}">
+    <text>Mute State Validation Issue Resolved with the help of Sahil on Bench 09, and the Appium issue resolved on Bench 06.</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2024-08-06T14:42:22.00" personId="{124407F7-A124-478C-91FF-291E9D96DE6A}" id="{22B59C60-CA0F-476C-B8F5-61A5244C0E0A}">
+    <text xml:space="preserve">
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,7 +817,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -828,7 +913,7 @@
     <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="12">
         <f>SUM(C2:C11)</f>
@@ -838,18 +923,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>SEARCH("In-Progress", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>SEARCH("Incomplete", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>SEARCH("Completed", D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11" xr:uid="{D817713A-50D7-4DD2-810F-8BB4A514456D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Completed, Incomplete, In-Progress"</formula1>
     </dataValidation>
   </dataValidations>
@@ -883,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -892,11 +977,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -905,11 +990,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -918,11 +1003,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -931,11 +1016,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -944,11 +1029,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -957,11 +1042,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -970,11 +1055,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1007,7 +1092,7 @@
     <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="12">
         <f>SUM(C2:C11)</f>
@@ -1017,13 +1102,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>SEARCH("In-Progress", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>SEARCH("Incomplete", D1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>SEARCH("Completed", D1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1057,7 +1142,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1066,11 +1151,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1079,11 +1164,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1092,11 +1177,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1105,11 +1190,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1118,11 +1203,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1131,11 +1216,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1144,11 +1229,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1157,11 +1242,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1170,11 +1255,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1183,11 +1268,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1196,23 +1281,191 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="6" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="12">
         <f>SUM(C2:C12)</f>
         <v>0</v>
       </c>
       <c r="D13" s="13"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>SEARCH("In-Progress", D1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>SEARCH("Incomplete", D1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>SEARCH("Completed", D1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="69.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <f t="shared" ref="A2:A11" si="0">ROW() - ROW($A$1)</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="12">
+        <f>SUM(C2:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
@@ -1226,16 +1479,21 @@
       <formula>SEARCH("Completed", D1)</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11" xr:uid="{00000000-0002-0000-0300-000000000000}">
+      <formula1>"Completed, Incomplete, In-Progress"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F135802-11A8-408F-949F-A2C0D125685D}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,7 +1514,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1265,11 +1523,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.5</v>
+      </c>
       <c r="D2" s="6" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1278,11 +1538,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1291,11 +1553,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1304,11 +1568,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1317,37 +1583,59 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="B8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="B9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -1355,10 +1643,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
@@ -1366,19 +1658,23 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="12">
         <f>SUM(C2:C11)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D12" s="13"/>
     </row>
@@ -1395,10 +1691,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11" xr:uid="{ED41C130-695A-4D4B-8B67-EE5F711418A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11" xr:uid="{AD3833FE-6D06-40F4-BE7F-755C8A684AD9}">
       <formula1>"Completed, Incomplete, In-Progress"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>